<commit_message>
Actualizacion casos de prueba
</commit_message>
<xml_diff>
--- a/Producto/Web/Casos de prueba/Resumen.xlsx
+++ b/Producto/Web/Casos de prueba/Resumen.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Nombre</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t>Buscar las playas esxistentes en una determinada ciudad, en la que no hay playas cargadas.</t>
+  </si>
+  <si>
+    <t>16_lucas</t>
+  </si>
+  <si>
+    <t>Buscar playas en una ciudad por tipo de vehiculo</t>
+  </si>
+  <si>
+    <t>Buscar las playas esxistentes en una determinada ciudad, por un tipo de vehiculo en particular</t>
   </si>
 </sst>
 </file>
@@ -259,7 +268,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -886,12 +895,12 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.28515625" customWidth="1"/>
     <col min="4" max="4" width="6.140625" customWidth="1"/>
@@ -1214,7 +1223,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1234,13 +1243,25 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -1363,9 +1384,10 @@
     <hyperlink ref="A14" r:id="rId13" display="13.xlsx"/>
     <hyperlink ref="A15" r:id="rId14" display="14 - lucas.xlsx"/>
     <hyperlink ref="A16" r:id="rId15" display="15 - lucas.xlsx"/>
+    <hyperlink ref="A17" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>